<commit_message>
Uploaded 12-Nov-2018 11:09:17 {/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx
+++ b/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx
@@ -58,22 +58,22 @@
     <t xml:space="preserve">program</t>
   </si>
   <si>
-    <t xml:space="preserve">$mortgage.lengthOfLoanYears &gt; $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$mortgage.lengthOfLoanYears &lt;= $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$mortgage.baseLoanAmount &gt;= $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$mortgage.baseLoanAmount &lt; $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$mortgage.ltv &gt;= $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$mortgage.ltv &lt; $param</t>
+    <t xml:space="preserve">lengthOfLoanYears &gt; $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lengthOfLoanYears &lt;= $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baseLoanAmount &gt;= $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baseLoanAmount &lt; $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ltv &gt;= $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ltv &lt; $param</t>
   </si>
   <si>
     <t xml:space="preserve">$mortgage.setAnnualMPI($param)</t>
@@ -148,6 +148,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -169,6 +170,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -240,23 +242,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,7 +350,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -357,58 +359,74 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -440,9 +458,16 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
@@ -470,32 +495,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+    <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 12-Nov-2018 11:20:07 {/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx
+++ b/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">ltv &lt; $param</t>
   </si>
   <si>
-    <t xml:space="preserve">$mortgage.setAnnualMIP($param)</t>
+    <t xml:space="preserve">$mortgage.setAnnualMIP($param);</t>
   </si>
   <si>
     <t xml:space="preserve">Rule Name</t>
@@ -349,8 +349,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Uploaded 12-Nov-2018 11:25:17 {/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx
+++ b/src/main/resources/com/redhat/bpms/example/pmi/PMI Spreadsheet.xlsx
@@ -233,7 +233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,7 +258,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,7 +366,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,42 +448,41 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3" t="s">
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
@@ -495,32 +510,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="10" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -528,26 +543,26 @@
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="G11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7" t="n">
+      <c r="B11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11" t="n">
         <v>90</v>
       </c>
-      <c r="I11" s="8" t="n">
+      <c r="I11" s="12" t="n">
         <v>45</v>
       </c>
     </row>
@@ -555,26 +570,26 @@
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="G12" s="7" t="n">
+      <c r="B12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E12" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="G12" s="11" t="n">
         <v>90</v>
       </c>
-      <c r="H12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8" t="n">
+      <c r="H12" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="n">
         <v>70</v>
       </c>
     </row>
@@ -582,26 +597,26 @@
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E13" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="7" t="n">
+      <c r="B13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11" t="n">
         <v>78</v>
       </c>
-      <c r="I13" s="8" t="n">
+      <c r="I13" s="12" t="n">
         <v>45</v>
       </c>
     </row>
@@ -609,26 +624,26 @@
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E14" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="F14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7" t="n">
+      <c r="B14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E14" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="F14" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11" t="n">
         <v>78</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="11" t="n">
         <v>90</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="I14" s="12" t="n">
         <v>70</v>
       </c>
     </row>
@@ -636,24 +651,24 @@
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E15" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="F15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7" t="n">
+      <c r="B15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E15" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="F15" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11" t="n">
         <v>90</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8" t="n">
+      <c r="H15" s="11"/>
+      <c r="I15" s="12" t="n">
         <v>95</v>
       </c>
     </row>
@@ -661,26 +676,26 @@
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7" t="n">
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="G16" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11" t="n">
         <v>95</v>
       </c>
-      <c r="I16" s="8" t="n">
+      <c r="I16" s="12" t="n">
         <v>80</v>
       </c>
     </row>
@@ -688,24 +703,24 @@
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="G17" s="7" t="n">
+      <c r="B17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="G17" s="11" t="n">
         <v>95</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8" t="n">
+      <c r="H17" s="11"/>
+      <c r="I17" s="12" t="n">
         <v>85</v>
       </c>
     </row>
@@ -713,26 +728,26 @@
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="F18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7" t="n">
+      <c r="B18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11" t="n">
         <v>95</v>
       </c>
-      <c r="I18" s="8" t="n">
+      <c r="I18" s="12" t="n">
         <v>100</v>
       </c>
     </row>
@@ -740,24 +755,24 @@
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="n">
-        <v>625000</v>
-      </c>
-      <c r="F19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="7" t="n">
+      <c r="B19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11" t="n">
+        <v>625000</v>
+      </c>
+      <c r="F19" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="11" t="n">
         <v>95</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="8" t="n">
+      <c r="H19" s="11"/>
+      <c r="I19" s="12" t="n">
         <v>105</v>
       </c>
     </row>
@@ -768,7 +783,7 @@
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B8:H8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>